<commit_message>
Soil Compaction Desig 5
Soil Compaction Desig 5
</commit_message>
<xml_diff>
--- a/Civilworks cost/Soil Compaction/Input.xlsx
+++ b/Civilworks cost/Soil Compaction/Input.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
+    <sheet name="Output_summary" sheetId="2" r:id="rId2"/>
+    <sheet name="Output_Details" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -27,24 +29,12 @@
     <t>value</t>
   </si>
   <si>
-    <t>gamma</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
     <t>ton/cum</t>
   </si>
   <si>
-    <t>Hi</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>sigmanot</t>
-  </si>
-  <si>
     <t>ton/sqm</t>
   </si>
   <si>
@@ -54,10 +44,94 @@
     <t>percent</t>
   </si>
   <si>
-    <t>conatact_width</t>
-  </si>
-  <si>
     <t>meter</t>
+  </si>
+  <si>
+    <t>Roller Type</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>gammanot</t>
+  </si>
+  <si>
+    <t>initial dry density</t>
+  </si>
+  <si>
+    <t>ton</t>
+  </si>
+  <si>
+    <t>Roller Weight</t>
+  </si>
+  <si>
+    <t>drum dia</t>
+  </si>
+  <si>
+    <t>drum length</t>
+  </si>
+  <si>
+    <t>tire pressure</t>
+  </si>
+  <si>
+    <t>1:Pneumatic 2:Smooth Wheel 3:Grid Roller 4:Sheepfoot Roller 5:Vibratory Roller</t>
+  </si>
+  <si>
+    <t>covearge ratio</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>0.5 for Grid Roller, 0.8-0.12 for sheepfoot roller</t>
+  </si>
+  <si>
+    <t>gammafinal</t>
+  </si>
+  <si>
+    <t>Max Lift Thickness</t>
+  </si>
+  <si>
+    <t>No of Passes</t>
+  </si>
+  <si>
+    <t>Ulitmate Bearing Capacity</t>
+  </si>
+  <si>
+    <t>Roller Adequecy</t>
+  </si>
+  <si>
+    <t>Sigmanot</t>
+  </si>
+  <si>
+    <t>Design Parameter</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Nos</t>
+  </si>
+  <si>
+    <t>Pass No</t>
+  </si>
+  <si>
+    <t>Gamma_initial</t>
+  </si>
+  <si>
+    <t>Lift thickness</t>
+  </si>
+  <si>
+    <t>Elastic modulus</t>
+  </si>
+  <si>
+    <t>Effective Depth</t>
+  </si>
+  <si>
+    <t>Final Lift Thickness</t>
+  </si>
+  <si>
+    <t>Gamma Final</t>
   </si>
 </sst>
 </file>
@@ -113,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -124,6 +198,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,82 +482,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5706</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>41.4</v>
-      </c>
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.5706</v>
-      </c>
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.36</v>
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>